<commit_message>
Changed how sites are grouped (now by filename, not split_by_site)
</commit_message>
<xml_diff>
--- a/qpcr_analyzer/sites.xlsx
+++ b/qpcr_analyzer/sites.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinwellman/Documents/Health/Wastewater/Code/qpcr_analyzer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinwellman/Documents/Health/Wastewater/Code/odm-qpcr-analyzer/qpcr_analyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48653B13-0339-0943-8473-33AD828BEB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A562F1F8-278E-E94A-9416-E5A2F786296C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{79FF871A-AFC0-EF4C-87C4-992B268ED25F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{79FF871A-AFC0-EF4C-87C4-992B268ED25F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="73">
   <si>
     <t>Site ID</t>
   </si>
@@ -138,12 +138,6 @@
     <t>VC3</t>
   </si>
   <si>
-    <t>Site Region</t>
-  </si>
-  <si>
-    <t>Site Location</t>
-  </si>
-  <si>
     <t>Type of Sample</t>
   </si>
   <si>
@@ -247,13 +241,16 @@
   </si>
   <si>
     <t>AwSt</t>
+  </si>
+  <si>
+    <t>Site Title</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -286,13 +283,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -314,14 +304,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,543 +625,479 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0A37EA-3BF4-7645-8CF0-89AEE0C49D57}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="4"/>
     <col min="2" max="2" width="50.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="10.83203125" style="4"/>
-    <col min="6" max="6" width="28" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="4"/>
+    <col min="3" max="3" width="15" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="4"/>
+    <col min="5" max="5" width="28" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>8</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="E6" s="1" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>8</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="E7" s="1" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>13</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>13</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>17</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>17</v>
+      <c r="F10" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" s="5" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="F11" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="F12" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="F14" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="F15" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>30</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>30</v>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>30</v>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="5" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="5" t="s">
+      <c r="C21" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>22</v>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5" t="s">
-        <v>60</v>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>22</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="E25" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Handle empty rows in updater, improved handling of unknown genes in extracter
</commit_message>
<xml_diff>
--- a/qpcr_analyzer/sites.xlsx
+++ b/qpcr_analyzer/sites.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinwellman/Documents/Health/Wastewater/Code/odm-qpcr-analyzer/qpcr_analyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A562F1F8-278E-E94A-9416-E5A2F786296C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDE5532-5165-634E-B334-CE41DE55D019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{79FF871A-AFC0-EF4C-87C4-992B268ED25F}"/>
+    <workbookView xWindow="12120" yWindow="500" windowWidth="16680" windowHeight="16040" xr2:uid="{79FF871A-AFC0-EF4C-87C4-992B268ED25F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateCount="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="86">
   <si>
     <t>Site ID</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Ham</t>
   </si>
   <si>
-    <t>Ham_MH</t>
-  </si>
-  <si>
     <t>Site ID Aliases</t>
   </si>
   <si>
@@ -244,13 +241,55 @@
   </si>
   <si>
     <t>Site Title</t>
+  </si>
+  <si>
+    <t>UONA</t>
+  </si>
+  <si>
+    <t>UOST</t>
+  </si>
+  <si>
+    <t>UOFA</t>
+  </si>
+  <si>
+    <t>UOAA</t>
+  </si>
+  <si>
+    <t>UOFT</t>
+  </si>
+  <si>
+    <t>UOSP</t>
+  </si>
+  <si>
+    <t>UONP</t>
+  </si>
+  <si>
+    <t>UONT</t>
+  </si>
+  <si>
+    <t>H_D</t>
+  </si>
+  <si>
+    <t>Dundas WWTP</t>
+  </si>
+  <si>
+    <t>HD</t>
+  </si>
+  <si>
+    <t>Ham_MH,HMH,H_MH</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Arbour Creek</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -283,6 +322,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -304,13 +354,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,17 +677,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0A37EA-3BF4-7645-8CF0-89AEE0C49D57}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="4"/>
-    <col min="2" max="2" width="50.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="4"/>
     <col min="5" max="5" width="28" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
@@ -647,10 +699,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>55</v>
@@ -800,7 +852,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>14</v>
@@ -814,84 +866,88 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="D10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>22</v>
+        <v>57</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>22</v>
+        <v>57</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>58</v>
       </c>
@@ -904,12 +960,14 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="D15" s="1" t="s">
         <v>58</v>
       </c>
@@ -922,12 +980,14 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>58</v>
       </c>
@@ -940,19 +1000,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>30</v>
+        <v>58</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>61</v>
@@ -960,19 +1020,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>30</v>
+        <v>58</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>61</v>
@@ -980,13 +1040,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>59</v>
@@ -999,104 +1059,150 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="5" t="s">
+      <c r="C22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1" t="s">
+      <c r="C25" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Outlier in Ottawa Wide template default changed to FALSE
</commit_message>
<xml_diff>
--- a/qpcr_analyzer/sites.xlsx
+++ b/qpcr_analyzer/sites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinwellman/Documents/Health/Wastewater/Code/odm-qpcr-analyzer/qpcr_analyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5580EF3E-E05D-D44D-8447-497DC80078BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA10C8F-462D-014B-AC0F-7AE23F2450BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="16680" windowHeight="16040" xr2:uid="{79FF871A-AFC0-EF4C-87C4-992B268ED25F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28620" windowHeight="16040" xr2:uid="{79FF871A-AFC0-EF4C-87C4-992B268ED25F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -683,7 +683,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,7 +694,8 @@
     <col min="4" max="4" width="10.83203125" style="4"/>
     <col min="5" max="5" width="28" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="4"/>
+    <col min="7" max="7" width="16.5" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -896,7 +897,7 @@
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>86</v>

</xml_diff>